<commit_message>
added mutable tables to model, deleted doc dictionary, added excel dictionary
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="1840" windowWidth="25800" windowHeight="18180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="297">
   <si>
     <t>id_review_dim</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1032,19 +1032,28 @@
   </si>
   <si>
     <t>location_dim</t>
+  </si>
+  <si>
+    <t>race_note</t>
+  </si>
+  <si>
+    <t>ethnicity_note</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Note about race - ex. Source, etc.</t>
+  </si>
+  <si>
+    <t>Note about ethnicity - ex. Source, etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1076,6 +1085,18 @@
       <sz val="14"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1085,7 +1106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1095,14 +1116,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1110,33 +1131,70 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1145,104 +1203,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color indexed="22"/>
@@ -1252,10 +1213,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color indexed="22"/>
@@ -1264,10 +1225,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1287,7 +1248,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color indexed="22"/>
@@ -1304,47 +1265,122 @@
         <color indexed="22"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color indexed="22"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1355,66 +1391,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1737,14 +1738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1757,1459 +1758,1455 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="24">
-      <c r="A4" s="21"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="21"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="21"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="24">
-      <c r="A8" s="21"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="24">
-      <c r="A9" s="21"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="21"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="21"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="21"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="21"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="17"/>
+      <c r="B14" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="17"/>
+      <c r="B15" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="20" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="21"/>
-      <c r="B15" s="13" t="s">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="17"/>
+      <c r="B17" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C17" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="21"/>
-      <c r="B17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="17"/>
+      <c r="B19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G19" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="21"/>
-      <c r="B18" s="10" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="17"/>
+      <c r="B20" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G20" s="8" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="24">
-      <c r="A19" s="21"/>
-      <c r="B19" s="13" t="s">
+    <row r="21" spans="1:7" ht="24">
+      <c r="A21" s="17"/>
+      <c r="B21" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="20" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="21"/>
-      <c r="B21" s="13" t="s">
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="17"/>
+      <c r="B23" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C23" s="10" t="s">
         <v>216</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="21"/>
-      <c r="B23" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="17"/>
+      <c r="B25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G25" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="21"/>
-      <c r="B24" s="10" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="17"/>
+      <c r="B26" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C26" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G26" s="8" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="24">
-      <c r="A25" s="21"/>
-      <c r="B25" s="13" t="s">
+    <row r="27" spans="1:7" ht="24">
+      <c r="A27" s="17"/>
+      <c r="B27" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C27" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13" t="s">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="20" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C28" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="21"/>
-      <c r="B27" s="13" t="s">
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="17"/>
+      <c r="B29" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C29" s="12" t="s">
         <v>221</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="24">
-      <c r="A28" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="21"/>
-      <c r="B29" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" ht="24">
+      <c r="A30" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="17"/>
+      <c r="B31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G31" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="21"/>
-      <c r="B30" s="10" t="s">
+    <row r="32" spans="1:7">
+      <c r="A32" s="17"/>
+      <c r="B32" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C32" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10" t="s">
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F32" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G32" s="8" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="24">
-      <c r="A31" s="21"/>
-      <c r="B31" s="13" t="s">
+    <row r="33" spans="1:7" ht="24">
+      <c r="A33" s="17"/>
+      <c r="B33" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C33" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13" t="s">
+      <c r="D33" s="10"/>
+      <c r="E33" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="20" t="s">
+      <c r="F33" s="10"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C34" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F34" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="21"/>
-      <c r="B33" s="13" t="s">
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="17"/>
+      <c r="B35" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C35" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="24">
-      <c r="A34" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="21"/>
-      <c r="B35" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" ht="24">
+      <c r="A36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="17"/>
+      <c r="B37" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G37" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="21"/>
-      <c r="B36" s="10" t="s">
+    <row r="38" spans="1:7">
+      <c r="A38" s="17"/>
+      <c r="B38" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C38" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10" t="s">
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G38" s="8" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="24">
-      <c r="A37" s="21"/>
-      <c r="B37" s="13" t="s">
+    <row r="39" spans="1:7" ht="24">
+      <c r="A39" s="17"/>
+      <c r="B39" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C39" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="21"/>
-      <c r="B39" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="21"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="17"/>
+      <c r="B41" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="17"/>
+      <c r="B42" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C42" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10" t="s">
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="21"/>
-      <c r="B41" s="10" t="s">
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="17"/>
+      <c r="B43" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C43" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10" t="s">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="11"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="21"/>
-      <c r="B42" s="10" t="s">
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="17"/>
+      <c r="B44" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C44" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10" t="s">
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="11"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="21"/>
-      <c r="B43" s="13" t="s">
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="17"/>
+      <c r="B45" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C45" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="15"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="9"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="21"/>
-      <c r="B45" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="21"/>
-      <c r="B46" s="10" t="s">
+      <c r="A46" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="17"/>
+      <c r="B47" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="17"/>
+      <c r="B48" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C48" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10" t="s">
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="21"/>
-      <c r="B47" s="10" t="s">
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="17"/>
+      <c r="B49" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C49" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10" t="s">
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F47" s="10"/>
-      <c r="G47" s="11"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="21"/>
-      <c r="B48" s="10" t="s">
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="17"/>
+      <c r="B50" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C50" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10" t="s">
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="10"/>
-      <c r="G48" s="11"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="21"/>
-      <c r="B49" s="10" t="s">
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="17"/>
+      <c r="B51" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C51" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10" t="s">
+      <c r="D51" s="7"/>
+      <c r="E51" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F49" s="10"/>
-      <c r="G49" s="11"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="21"/>
-      <c r="B50" s="10" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="17"/>
+      <c r="B52" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C52" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10" t="s">
+      <c r="D52" s="7"/>
+      <c r="E52" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="11"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="21"/>
-      <c r="B51" s="13" t="s">
+      <c r="F52" s="7"/>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="17"/>
+      <c r="B53" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C53" s="10" t="s">
         <v>160</v>
-      </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="24">
-      <c r="A52" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G52" s="9"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="21"/>
-      <c r="B53" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="11"/>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="21"/>
-      <c r="B54" s="10" t="s">
+      <c r="F53" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="24">
+      <c r="A54" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="17"/>
+      <c r="B55" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="17"/>
+      <c r="B56" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C56" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10" t="s">
+      <c r="D56" s="7"/>
+      <c r="E56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="10"/>
-      <c r="G54" s="11"/>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="21"/>
-      <c r="B55" s="10" t="s">
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="17"/>
+      <c r="B57" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C57" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10" t="s">
+      <c r="D57" s="7"/>
+      <c r="E57" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="10"/>
-      <c r="G55" s="11"/>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="21"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="17" t="s">
+      <c r="F57" s="7"/>
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="17"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="15"/>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G57" s="9"/>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="21"/>
-      <c r="B58" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>167</v>
-      </c>
       <c r="D58" s="10"/>
-      <c r="E58" s="18" t="s">
-        <v>31</v>
-      </c>
+      <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7" ht="24">
-      <c r="A59" s="21"/>
-      <c r="B59" s="13" t="s">
+    <row r="59" spans="1:7">
+      <c r="A59" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="17"/>
+      <c r="B60" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" ht="24">
+      <c r="A61" s="17"/>
+      <c r="B61" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C61" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" s="13"/>
-      <c r="G59" s="15"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G60" s="9"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="21"/>
-      <c r="B61" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="10" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="21"/>
-      <c r="B62" s="13" t="s">
+      <c r="A62" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="17"/>
+      <c r="B63" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="17"/>
+      <c r="B64" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C64" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="13"/>
-      <c r="G62" s="15"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G63" s="9"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="21"/>
-      <c r="B64" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>3</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="11"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="21"/>
-      <c r="B65" s="10" t="s">
+      <c r="A65" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="17"/>
+      <c r="B66" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="17"/>
+      <c r="B67" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C67" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10" t="s">
+      <c r="D67" s="7"/>
+      <c r="E67" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F65" s="10"/>
-      <c r="G65" s="11"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="21"/>
-      <c r="B66" s="13" t="s">
+      <c r="F67" s="7"/>
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="17"/>
+      <c r="B68" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C68" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="13"/>
-      <c r="G66" s="15"/>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G67" s="9"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="21"/>
-      <c r="B68" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="11"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="21"/>
-      <c r="B69" s="10" t="s">
+      <c r="A69" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="17"/>
+      <c r="B70" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="17"/>
+      <c r="B71" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C71" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10" t="s">
+      <c r="D71" s="7"/>
+      <c r="E71" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F69" s="10"/>
-      <c r="G69" s="11"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="21"/>
-      <c r="B70" s="10" t="s">
+      <c r="F71" s="7"/>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="17"/>
+      <c r="B72" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C72" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10" t="s">
+      <c r="D72" s="7"/>
+      <c r="E72" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="11"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="21"/>
-      <c r="B71" s="13" t="s">
+      <c r="F72" s="7"/>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="17"/>
+      <c r="B73" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C73" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F71" s="13"/>
-      <c r="G71" s="15"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G72" s="9"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="21"/>
-      <c r="B73" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>5</v>
       </c>
       <c r="D73" s="10"/>
       <c r="E73" s="10" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F73" s="10"/>
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="21"/>
-      <c r="B74" s="10" t="s">
+      <c r="A74" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="17"/>
+      <c r="B75" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="17"/>
+      <c r="B76" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C76" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10" t="s">
+      <c r="D76" s="7"/>
+      <c r="E76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F74" s="10"/>
-      <c r="G74" s="11"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="21"/>
-      <c r="B75" s="10" t="s">
+      <c r="F76" s="7"/>
+      <c r="G76" s="8"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="17"/>
+      <c r="B77" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C77" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10" t="s">
+      <c r="D77" s="7"/>
+      <c r="E77" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F75" s="10"/>
-      <c r="G75" s="11"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="21"/>
-      <c r="B76" s="10" t="s">
+      <c r="F77" s="7"/>
+      <c r="G77" s="8"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="17"/>
+      <c r="B78" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C78" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10" t="s">
+      <c r="D78" s="7"/>
+      <c r="E78" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F76" s="10"/>
-      <c r="G76" s="11"/>
-    </row>
-    <row r="77" spans="1:7" ht="24">
-      <c r="A77" s="21"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="19" t="s">
+      <c r="F78" s="7"/>
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" spans="1:7" ht="24">
+      <c r="A79" s="17"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="11"/>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="21"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="17" t="s">
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="17"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="15"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G79" s="9"/>
-    </row>
-    <row r="80" spans="1:7" ht="24">
-      <c r="A80" s="21"/>
-      <c r="B80" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>130</v>
-      </c>
       <c r="D80" s="10"/>
-      <c r="E80" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="E80" s="10"/>
       <c r="F80" s="10"/>
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="21"/>
-      <c r="B81" s="10" t="s">
+      <c r="A81" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82" spans="1:7" ht="24">
+      <c r="A82" s="17"/>
+      <c r="B82" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="7"/>
+      <c r="G82" s="8"/>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="17"/>
+      <c r="B83" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C83" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10" t="s">
+      <c r="D83" s="7"/>
+      <c r="E83" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F81" s="10"/>
-      <c r="G81" s="11"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="21"/>
-      <c r="B82" s="13" t="s">
+      <c r="F83" s="7"/>
+      <c r="G83" s="8"/>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="17"/>
+      <c r="B84" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C84" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F82" s="13"/>
-      <c r="G82" s="15"/>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G83" s="9"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="21"/>
-      <c r="B84" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="11"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="21"/>
-      <c r="B85" s="13" t="s">
+      <c r="A85" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="17"/>
+      <c r="B86" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="8"/>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="17"/>
+      <c r="B87" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C87" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="13"/>
-      <c r="G85" s="15"/>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G86" s="9"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="21"/>
-      <c r="B87" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="10" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F87" s="10"/>
       <c r="G87" s="11"/>
     </row>
-    <row r="88" spans="1:7" ht="24">
-      <c r="A88" s="21"/>
-      <c r="B88" s="13" t="s">
+    <row r="88" spans="1:7">
+      <c r="A88" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="17"/>
+      <c r="B89" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="8"/>
+    </row>
+    <row r="90" spans="1:7" ht="24">
+      <c r="A90" s="17"/>
+      <c r="B90" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C90" s="10" t="s">
         <v>138</v>
-      </c>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F88" s="13"/>
-      <c r="G88" s="15"/>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G89" s="9"/>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="21"/>
-      <c r="B90" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="D90" s="10"/>
       <c r="E90" s="10" t="s">
@@ -3219,348 +3216,382 @@
       <c r="G90" s="11"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="21"/>
-      <c r="B91" s="13" t="s">
+      <c r="A91" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="17"/>
+      <c r="B92" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="8"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="17"/>
+      <c r="B93" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C93" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F91" s="13"/>
-      <c r="G91" s="15"/>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G92" s="9"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="21"/>
-      <c r="B93" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" s="10"/>
+      <c r="G93" s="11"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="17"/>
+      <c r="B95" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="F95" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G93" s="11" t="s">
+      <c r="G95" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="21"/>
-      <c r="B94" s="10" t="s">
+    <row r="96" spans="1:7">
+      <c r="A96" s="17"/>
+      <c r="B96" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C96" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10" t="s">
+      <c r="D96" s="7"/>
+      <c r="E96" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="F96" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G94" s="11" t="s">
+      <c r="G96" s="8" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
-      <c r="A95" s="21"/>
-      <c r="B95" s="10" t="s">
+    <row r="97" spans="1:7">
+      <c r="A97" s="17"/>
+      <c r="B97" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="C97" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10" t="s">
+      <c r="D97" s="7"/>
+      <c r="E97" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F95" s="10" t="s">
+      <c r="F97" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G95" s="11" t="s">
+      <c r="G97" s="8" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
-      <c r="A96" s="21"/>
-      <c r="B96" s="10" t="s">
+    <row r="98" spans="1:7">
+      <c r="A98" s="17"/>
+      <c r="B98" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C98" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10" t="s">
+      <c r="D98" s="7"/>
+      <c r="E98" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="F98" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G96" s="11" t="s">
+      <c r="G98" s="8" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="21"/>
-      <c r="B97" s="10" t="s">
+    <row r="99" spans="1:7">
+      <c r="A99" s="17"/>
+      <c r="B99" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C99" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10" t="s">
+      <c r="D99" s="7"/>
+      <c r="E99" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="F99" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G97" s="11" t="s">
+      <c r="G99" s="8" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
-      <c r="A98" s="21"/>
-      <c r="B98" s="10" t="s">
+    <row r="100" spans="1:7">
+      <c r="A100" s="17"/>
+      <c r="B100" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C98" s="10" t="s">
+      <c r="C100" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10" t="s">
+      <c r="D100" s="7"/>
+      <c r="E100" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F98" s="10" t="s">
+      <c r="F100" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G98" s="11" t="s">
+      <c r="G100" s="8" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
-      <c r="A99" s="21"/>
-      <c r="B99" s="10" t="s">
+    <row r="101" spans="1:7">
+      <c r="A101" s="17"/>
+      <c r="B101" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C101" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10" t="s">
+      <c r="D101" s="7"/>
+      <c r="E101" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F99" s="10" t="s">
+      <c r="F101" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G99" s="11" t="s">
+      <c r="G101" s="8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="21"/>
-      <c r="B100" s="10" t="s">
+    <row r="102" spans="1:7">
+      <c r="A102" s="17"/>
+      <c r="B102" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C100" s="10" t="s">
+      <c r="C102" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10" t="s">
+      <c r="D102" s="7"/>
+      <c r="E102" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F100" s="10" t="s">
+      <c r="F102" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G100" s="11" t="s">
+      <c r="G102" s="8" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="21"/>
-      <c r="B101" s="10" t="s">
+    <row r="103" spans="1:7">
+      <c r="A103" s="17"/>
+      <c r="B103" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C101" s="10" t="s">
+      <c r="C103" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10" t="s">
+      <c r="D103" s="7"/>
+      <c r="E103" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F101" s="10" t="s">
+      <c r="F103" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G101" s="11" t="s">
+      <c r="G103" s="8" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="21"/>
-      <c r="B102" s="10" t="s">
+    <row r="104" spans="1:7">
+      <c r="A104" s="17"/>
+      <c r="B104" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="C104" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10" t="s">
+      <c r="D104" s="7"/>
+      <c r="E104" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F102" s="10" t="s">
+      <c r="F104" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G102" s="11" t="s">
+      <c r="G104" s="8" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="21"/>
-      <c r="B103" s="10" t="s">
+    <row r="105" spans="1:7">
+      <c r="A105" s="17"/>
+      <c r="B105" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C103" s="10" t="s">
+      <c r="C105" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D103" s="10"/>
-      <c r="E103" s="10" t="s">
+      <c r="D105" s="7"/>
+      <c r="E105" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F103" s="10" t="s">
+      <c r="F105" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G103" s="11" t="s">
+      <c r="G105" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="21"/>
-      <c r="B104" s="10" t="s">
+    <row r="106" spans="1:7">
+      <c r="A106" s="17"/>
+      <c r="B106" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C106" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10" t="s">
+      <c r="D106" s="7"/>
+      <c r="E106" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F104" s="10" t="s">
+      <c r="F106" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G104" s="11" t="s">
+      <c r="G106" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="21"/>
-      <c r="B105" s="10" t="s">
+    <row r="107" spans="1:7">
+      <c r="A107" s="17"/>
+      <c r="B107" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C105" s="10" t="s">
+      <c r="C107" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10" t="s">
+      <c r="D107" s="7"/>
+      <c r="E107" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F105" s="10" t="s">
+      <c r="F107" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G105" s="11" t="s">
+      <c r="G107" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="21"/>
-      <c r="B106" s="10" t="s">
+    <row r="108" spans="1:7">
+      <c r="A108" s="17"/>
+      <c r="B108" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C108" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10" t="s">
+      <c r="D108" s="7"/>
+      <c r="E108" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F106" s="10" t="s">
+      <c r="F108" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G106" s="11" t="s">
+      <c r="G108" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="21"/>
-      <c r="B107" s="10" t="s">
+    <row r="109" spans="1:7">
+      <c r="A109" s="17"/>
+      <c r="B109" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C107" s="10" t="s">
+      <c r="C109" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10" t="s">
+      <c r="D109" s="7"/>
+      <c r="E109" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F107" s="10" t="s">
+      <c r="F109" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G107" s="11" t="s">
+      <c r="G109" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="22"/>
-      <c r="B108" s="13" t="s">
+    <row r="110" spans="1:7">
+      <c r="A110" s="18"/>
+      <c r="B110" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C110" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13" t="s">
+      <c r="D110" s="10"/>
+      <c r="E110" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F108" s="13" t="s">
+      <c r="F110" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G108" s="15" t="s">
+      <c r="G110" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="1" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B113" s="2">
         <v>40739</v>
       </c>
     </row>
@@ -3572,7 +3603,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>